<commit_message>
get formatting data in dataframe dictionary so we can access format data from specific cells
</commit_message>
<xml_diff>
--- a/openpyxl/format_test.xlsx
+++ b/openpyxl/format_test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nellie/Documenten/Python_programs/masterproef/xlwings/unittests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nellie/Documenten/Python_programs/masterproef/openpyxl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78178DF6-7FB9-434E-818E-590E0FF0624E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20F01DC-A3BD-E14B-A2DC-5351FE9CA7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="500" windowWidth="19560" windowHeight="16120" xr2:uid="{FD6B2ABE-307B-7749-B34E-24325EB3B4E8}"/>
+    <workbookView xWindow="17340" yWindow="500" windowWidth="11460" windowHeight="16120" activeTab="1" xr2:uid="{FD6B2ABE-307B-7749-B34E-24325EB3B4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,9 +37,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="1">
-  <si>
-    <t>hello</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>fff</t>
+  </si>
+  <si>
+    <t>ggg</t>
+  </si>
+  <si>
+    <t>hhh</t>
+  </si>
+  <si>
+    <t>iii</t>
+  </si>
+  <si>
+    <t>jjj</t>
+  </si>
+  <si>
+    <t>kkk</t>
+  </si>
+  <si>
+    <t>llll</t>
+  </si>
+  <si>
+    <t>mmmm</t>
+  </si>
+  <si>
+    <t>nnnn</t>
+  </si>
+  <si>
+    <t>oooo</t>
+  </si>
+  <si>
+    <t>pppp</t>
   </si>
 </sst>
 </file>
@@ -173,7 +219,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +564,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CF53EA-F9F1-B548-A42D-FB0112CF5199}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -529,52 +577,86 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E150EF6F-546B-2A45-A082-D2D8080E0D2F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formatting is properly being read out (MacOS and Windows), using xlwings for correct retrieval of text- and cell colors
</commit_message>
<xml_diff>
--- a/openpyxl/format_test.xlsx
+++ b/openpyxl/format_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nellie/Documenten/Python_programs/masterproef/openpyxl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20F01DC-A3BD-E14B-A2DC-5351FE9CA7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE610DA-6F54-3A4F-9BBD-F29D5B170074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="500" windowWidth="11460" windowHeight="16120" activeTab="1" xr2:uid="{FD6B2ABE-307B-7749-B34E-24325EB3B4E8}"/>
+    <workbookView xWindow="-14200" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{FD6B2ABE-307B-7749-B34E-24325EB3B4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,48 +130,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="12"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF00FA00"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <strike/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="12"/>
-      <color theme="5"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -208,18 +215,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -228,10 +236,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FA00"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF0432FF"/>
       <color rgb="FF00FDFF"/>
-      <color rgb="FF00FA00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -564,14 +572,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CF53EA-F9F1-B548-A42D-FB0112CF5199}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
@@ -581,7 +589,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -591,22 +599,22 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -616,12 +624,12 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -634,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E150EF6F-546B-2A45-A082-D2D8080E0D2F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>